<commit_message>
Final updates from WRI on Hong Kong model
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22223"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipP\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3f05\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D1D127A6F92FA3437A4AED662F748F1322AC704B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_D1D127A6F92FA3437A4AED662F748F1322AC704B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9418616E-59B7-4DDF-B181-6B34FEF9E000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18180" windowHeight="8730" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25560" windowHeight="15060" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
     <sheet name="Key to Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Key to Top Level Folders" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Key to Variables'!$A$1:$G$189</definedName>
+  </definedNames>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1677,7 +1680,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2190,82 +2193,82 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>14</v>
       </c>
@@ -2273,32 +2276,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>21</v>
       </c>
@@ -2306,17 +2309,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>25</v>
       </c>
@@ -2324,42 +2327,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>34</v>
       </c>
@@ -2367,84 +2370,84 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>51</v>
       </c>
@@ -2452,62 +2455,62 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -2520,14 +2523,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="2" customWidth="1"/>
@@ -2539,7 +2543,7 @@
     <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>65</v>
       </c>
@@ -2562,7 +2566,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -2576,7 +2580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -2593,7 +2597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1">
+    <row r="4" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>72</v>
       </c>
@@ -2610,7 +2614,7 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>79</v>
       </c>
@@ -2624,7 +2628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
@@ -2655,7 +2659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>79</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="13" customFormat="1" ht="45" customHeight="1">
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
@@ -2689,7 +2693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>79</v>
       </c>
@@ -2703,7 +2707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
@@ -2717,9 +2721,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>276</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>98</v>
@@ -2731,7 +2735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>79</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>79</v>
       </c>
@@ -2759,7 +2763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>79</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>79</v>
       </c>
@@ -2801,7 +2805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>79</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>79</v>
       </c>
@@ -2832,7 +2836,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>79</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30">
+    <row r="22" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30">
+    <row r="23" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
@@ -2891,7 +2895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45">
+    <row r="24" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30.75" thickBot="1">
+    <row r="25" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>79</v>
       </c>
@@ -2925,7 +2929,7 @@
       </c>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>128</v>
       </c>
@@ -2942,7 +2946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>128</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>128</v>
       </c>
@@ -2978,7 +2982,7 @@
       </c>
       <c r="G28" s="19"/>
     </row>
-    <row r="29" spans="1:7" ht="30">
+    <row r="29" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>138</v>
       </c>
@@ -2995,7 +2999,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1">
+    <row r="30" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>138</v>
       </c>
@@ -3012,7 +3016,7 @@
       </c>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>144</v>
       </c>
@@ -3026,7 +3030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>144</v>
       </c>
@@ -3040,7 +3044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="28" customFormat="1">
+    <row r="33" spans="1:7" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>144</v>
       </c>
@@ -3054,7 +3058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="30" customFormat="1" ht="30.75" thickBot="1">
+    <row r="34" spans="1:7" s="30" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>144</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>154</v>
       </c>
@@ -3087,7 +3091,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>154</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>154</v>
       </c>
@@ -3115,7 +3119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="45">
+    <row r="38" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>154</v>
       </c>
@@ -3132,7 +3136,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>154</v>
       </c>
@@ -3146,7 +3150,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>154</v>
       </c>
@@ -3160,7 +3164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>154</v>
       </c>
@@ -3174,7 +3178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>154</v>
       </c>
@@ -3188,7 +3192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="45">
+    <row r="43" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>154</v>
       </c>
@@ -3205,7 +3209,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>154</v>
       </c>
@@ -3219,7 +3223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30">
+    <row r="45" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>154</v>
       </c>
@@ -3236,7 +3240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>154</v>
       </c>
@@ -3250,7 +3254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="75">
+    <row r="47" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>154</v>
       </c>
@@ -3267,7 +3271,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>154</v>
       </c>
@@ -3281,7 +3285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>154</v>
       </c>
@@ -3295,7 +3299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>154</v>
       </c>
@@ -3309,7 +3313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30">
+    <row r="51" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>154</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>154</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="60">
+    <row r="53" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>154</v>
       </c>
@@ -3357,7 +3361,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30">
+    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>154</v>
       </c>
@@ -3375,7 +3379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30">
+    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>154</v>
       </c>
@@ -3393,7 +3397,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>154</v>
       </c>
@@ -3410,7 +3414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>154</v>
       </c>
@@ -3424,7 +3428,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="30">
+    <row r="58" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>154</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="120">
+    <row r="59" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>154</v>
       </c>
@@ -3455,7 +3459,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>154</v>
       </c>
@@ -3469,7 +3473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="60">
+    <row r="61" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>154</v>
       </c>
@@ -3486,7 +3490,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>154</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>154</v>
       </c>
@@ -3514,7 +3518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>154</v>
       </c>
@@ -3528,7 +3532,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>154</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>154</v>
       </c>
@@ -3556,7 +3560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>154</v>
       </c>
@@ -3570,7 +3574,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="60">
+    <row r="68" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>154</v>
       </c>
@@ -3587,7 +3591,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>154</v>
       </c>
@@ -3601,7 +3605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>154</v>
       </c>
@@ -3615,7 +3619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30">
+    <row r="71" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>154</v>
       </c>
@@ -3632,7 +3636,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>154</v>
       </c>
@@ -3646,7 +3650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30">
+    <row r="73" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>154</v>
       </c>
@@ -3663,7 +3667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30">
+    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>154</v>
       </c>
@@ -3677,7 +3681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30">
+    <row r="75" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>154</v>
       </c>
@@ -3691,7 +3695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="60.75" thickBot="1">
+    <row r="76" spans="1:7" ht="60.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>154</v>
       </c>
@@ -3712,7 +3716,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>257</v>
       </c>
@@ -3726,7 +3730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>257</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>257</v>
       </c>
@@ -3754,7 +3758,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>257</v>
       </c>
@@ -3768,7 +3772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>257</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>257</v>
       </c>
@@ -3796,7 +3800,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30">
+    <row r="83" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>257</v>
       </c>
@@ -3810,7 +3814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30">
+    <row r="84" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>257</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1">
+    <row r="85" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
         <v>257</v>
       </c>
@@ -3841,7 +3845,7 @@
       </c>
       <c r="G85" s="19"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>276</v>
       </c>
@@ -3855,7 +3859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>276</v>
       </c>
@@ -3872,7 +3876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="45">
+    <row r="88" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>276</v>
       </c>
@@ -3889,7 +3893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>276</v>
       </c>
@@ -3903,7 +3907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="30">
+    <row r="90" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>276</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>276</v>
       </c>
@@ -3934,7 +3938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="30">
+    <row r="92" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>276</v>
       </c>
@@ -3951,7 +3955,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>276</v>
       </c>
@@ -3965,7 +3969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="30">
+    <row r="94" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>276</v>
       </c>
@@ -3982,7 +3986,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="30">
+    <row r="95" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>276</v>
       </c>
@@ -3999,7 +4003,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30">
+    <row r="96" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>276</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="45">
+    <row r="97" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>276</v>
       </c>
@@ -4033,7 +4037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="60">
+    <row r="98" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="28" t="s">
         <v>276</v>
       </c>
@@ -4052,7 +4056,7 @@
       </c>
       <c r="G98" s="28"/>
     </row>
-    <row r="99" spans="1:7" ht="30.75" thickBot="1">
+    <row r="99" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="19" t="s">
         <v>276</v>
       </c>
@@ -4069,7 +4073,7 @@
       </c>
       <c r="G99" s="19"/>
     </row>
-    <row r="100" spans="1:7" s="13" customFormat="1">
+    <row r="100" spans="1:7" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>314</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="13" customFormat="1">
+    <row r="101" spans="1:7" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>314</v>
       </c>
@@ -4097,7 +4101,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="13" customFormat="1">
+    <row r="102" spans="1:7" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>314</v>
       </c>
@@ -4111,7 +4115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="13" customFormat="1" ht="30">
+    <row r="103" spans="1:7" s="13" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>314</v>
       </c>
@@ -4128,7 +4132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="13" customFormat="1" ht="30">
+    <row r="104" spans="1:7" s="13" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>314</v>
       </c>
@@ -4142,7 +4146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="13" customFormat="1">
+    <row r="105" spans="1:7" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>314</v>
       </c>
@@ -4159,7 +4163,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1">
+    <row r="106" spans="1:7" s="13" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
         <v>314</v>
       </c>
@@ -4178,7 +4182,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>332</v>
       </c>
@@ -4192,7 +4196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="30">
+    <row r="108" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>332</v>
       </c>
@@ -4212,7 +4216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="30">
+    <row r="109" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>332</v>
       </c>
@@ -4229,7 +4233,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="30">
+    <row r="110" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>332</v>
       </c>
@@ -4243,7 +4247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>332</v>
       </c>
@@ -4257,7 +4261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30">
+    <row r="112" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>332</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30">
+    <row r="113" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>332</v>
       </c>
@@ -4288,7 +4292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>332</v>
       </c>
@@ -4305,7 +4309,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="30">
+    <row r="115" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>332</v>
       </c>
@@ -4323,7 +4327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="30">
+    <row r="116" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>332</v>
       </c>
@@ -4339,7 +4343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>332</v>
       </c>
@@ -4353,7 +4357,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="30">
+    <row r="118" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>332</v>
       </c>
@@ -4373,7 +4377,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="30">
+    <row r="119" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>332</v>
       </c>
@@ -4387,7 +4391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30">
+    <row r="120" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>332</v>
       </c>
@@ -4401,7 +4405,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30">
+    <row r="121" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>332</v>
       </c>
@@ -4415,7 +4419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="30">
+    <row r="122" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>332</v>
       </c>
@@ -4429,7 +4433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="45">
+    <row r="123" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>332</v>
       </c>
@@ -4446,7 +4450,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="30">
+    <row r="124" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>332</v>
       </c>
@@ -4460,7 +4464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>332</v>
       </c>
@@ -4474,7 +4478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15.75" thickBot="1">
+    <row r="126" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="19" t="s">
         <v>332</v>
       </c>
@@ -4491,7 +4495,7 @@
       </c>
       <c r="G126" s="19"/>
     </row>
-    <row r="127" spans="1:7" ht="30">
+    <row r="127" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>381</v>
       </c>
@@ -4505,7 +4509,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>381</v>
       </c>
@@ -4522,7 +4526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="30">
+    <row r="129" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>381</v>
       </c>
@@ -4536,7 +4540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="30">
+    <row r="130" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>381</v>
       </c>
@@ -4553,7 +4557,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="30">
+    <row r="131" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>381</v>
       </c>
@@ -4567,7 +4571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>381</v>
       </c>
@@ -4581,7 +4585,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>381</v>
       </c>
@@ -4595,7 +4599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="30">
+    <row r="134" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>381</v>
       </c>
@@ -4609,7 +4613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="30">
+    <row r="135" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>381</v>
       </c>
@@ -4623,7 +4627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="30.75" thickBot="1">
+    <row r="136" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="19" t="s">
         <v>381</v>
       </c>
@@ -4640,7 +4644,7 @@
       </c>
       <c r="G136" s="19"/>
     </row>
-    <row r="137" spans="1:7" ht="60">
+    <row r="137" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>403</v>
       </c>
@@ -4657,7 +4661,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="45">
+    <row r="138" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>403</v>
       </c>
@@ -4674,7 +4678,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="60">
+    <row r="139" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>403</v>
       </c>
@@ -4691,7 +4695,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="60">
+    <row r="140" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>403</v>
       </c>
@@ -4708,7 +4712,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="30.75" thickBot="1">
+    <row r="141" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="19" t="s">
         <v>403</v>
       </c>
@@ -4727,7 +4731,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="30">
+    <row r="142" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>420</v>
       </c>
@@ -4744,7 +4748,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>420</v>
       </c>
@@ -4761,7 +4765,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="30.75" thickBot="1">
+    <row r="144" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="19" t="s">
         <v>420</v>
       </c>
@@ -4780,7 +4784,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>430</v>
       </c>
@@ -4794,7 +4798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>430</v>
       </c>
@@ -4808,7 +4812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>430</v>
       </c>
@@ -4822,7 +4826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="30">
+    <row r="148" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>430</v>
       </c>
@@ -4836,7 +4840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>430</v>
       </c>
@@ -4850,7 +4854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="30">
+    <row r="150" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>430</v>
       </c>
@@ -4867,7 +4871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>430</v>
       </c>
@@ -4881,7 +4885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>430</v>
       </c>
@@ -4895,7 +4899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>430</v>
       </c>
@@ -4909,7 +4913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="30">
+    <row r="154" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>430</v>
       </c>
@@ -4923,7 +4927,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>430</v>
       </c>
@@ -4937,7 +4941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>430</v>
       </c>
@@ -4951,7 +4955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>430</v>
       </c>
@@ -4965,7 +4969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="60">
+    <row r="158" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>430</v>
       </c>
@@ -4982,7 +4986,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>430</v>
       </c>
@@ -4996,7 +5000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>430</v>
       </c>
@@ -5010,7 +5014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>430</v>
       </c>
@@ -5024,7 +5028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>430</v>
       </c>
@@ -5038,7 +5042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>430</v>
       </c>
@@ -5052,7 +5056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>430</v>
       </c>
@@ -5066,7 +5070,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>430</v>
       </c>
@@ -5080,7 +5084,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>430</v>
       </c>
@@ -5094,7 +5098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>430</v>
       </c>
@@ -5108,7 +5112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="60">
+    <row r="168" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>430</v>
       </c>
@@ -5125,7 +5129,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="60">
+    <row r="169" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>430</v>
       </c>
@@ -5142,7 +5146,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="60">
+    <row r="170" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>430</v>
       </c>
@@ -5159,7 +5163,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>430</v>
       </c>
@@ -5176,7 +5180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>430</v>
       </c>
@@ -5193,7 +5197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>430</v>
       </c>
@@ -5207,7 +5211,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>430</v>
       </c>
@@ -5221,7 +5225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="30">
+    <row r="175" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>430</v>
       </c>
@@ -5235,7 +5239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>430</v>
       </c>
@@ -5252,7 +5256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>430</v>
       </c>
@@ -5266,7 +5270,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>430</v>
       </c>
@@ -5280,7 +5284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="30">
+    <row r="179" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>430</v>
       </c>
@@ -5294,7 +5298,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>430</v>
       </c>
@@ -5308,7 +5312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>430</v>
       </c>
@@ -5322,7 +5326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>430</v>
       </c>
@@ -5336,7 +5340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="60">
+    <row r="183" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>430</v>
       </c>
@@ -5353,7 +5357,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="30.75" thickBot="1">
+    <row r="184" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="19" t="s">
         <v>430</v>
       </c>
@@ -5370,7 +5374,7 @@
       </c>
       <c r="G184" s="19"/>
     </row>
-    <row r="185" spans="1:7" ht="45">
+    <row r="185" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>517</v>
       </c>
@@ -5387,7 +5391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>517</v>
       </c>
@@ -5401,7 +5405,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="30">
+    <row r="187" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>517</v>
       </c>
@@ -5418,7 +5422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>517</v>
       </c>
@@ -5432,7 +5436,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="30.75" thickBot="1">
+    <row r="189" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="19" t="s">
         <v>517</v>
       </c>
@@ -5452,6 +5456,13 @@
       <c r="G189" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G189" xr:uid="{8F1A0034-FB68-4E71-903A-F0F58E0F3790}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ccs"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -5466,13 +5477,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -5480,7 +5491,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -5488,7 +5499,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -5496,7 +5507,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -5504,7 +5515,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -5512,7 +5523,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -5520,7 +5531,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -5528,7 +5539,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -5536,7 +5547,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -5544,7 +5555,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>314</v>
       </c>
@@ -5552,7 +5563,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>332</v>
       </c>
@@ -5560,7 +5571,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>381</v>
       </c>
@@ -5568,7 +5579,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>403</v>
       </c>
@@ -5576,7 +5587,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>420</v>
       </c>
@@ -5584,7 +5595,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>430</v>
       </c>
@@ -5592,7 +5603,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>517</v>
       </c>
@@ -5615,15 +5626,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5857,14 +5859,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1B10BC-4FA1-4D78-BE87-050592A4192D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1B10BC-4FA1-4D78-BE87-050592A4192D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F984B1A-22E0-4FF6-9077-24DC55010239}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC686F6F-A43A-4F7E-81D0-BB9483096F8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC686F6F-A43A-4F7E-81D0-BB9483096F8E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F984B1A-22E0-4FF6-9077-24DC55010239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>